<commit_message>
add the different modules
</commit_message>
<xml_diff>
--- a/SE_LAB_2 TEST CASE FILE.xlsx
+++ b/SE_LAB_2 TEST CASE FILE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22170" windowHeight="10745"/>
+    <workbookView windowWidth="26083" windowHeight="10745"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,6 +138,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Grade: </t>
     </r>
     <r>
@@ -173,6 +180,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Grade: </t>
     </r>
     <r>
@@ -208,6 +222,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Grade: </t>
     </r>
     <r>
@@ -942,7 +963,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -953,9 +974,6 @@
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1238,9 +1256,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>635</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
@@ -1257,14 +1275,15 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
+        <a:srcRect t="2846"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3438525"/>
-          <a:ext cx="6635750" cy="5737860"/>
+          <a:off x="635" y="3602355"/>
+          <a:ext cx="6635115" cy="5574030"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1624,8 +1643,8 @@
   <sheetPr/>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99082568807339" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -1931,7 +1950,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="4"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6">
@@ -1939,7 +1958,7 @@
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="4"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
     <row r="40" spans="4:4">

</xml_diff>